<commit_message>
Ingestion data avvenuto correttamente
</commit_message>
<xml_diff>
--- a/turniMaker/src/main/resources/dati.xlsx
+++ b/turniMaker/src/main/resources/dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\turniMaker\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E445B4E5-FD8D-4EC2-B288-5FE741ADC273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F95661-B861-4B73-90DB-14CC3F5AD3F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="5595" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4425" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Persone-Indisp" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
   <si>
     <t>BAI</t>
   </si>
@@ -57,6 +57,30 @@
   </si>
   <si>
     <t>GN</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>MIG</t>
+  </si>
+  <si>
+    <t>FAN</t>
+  </si>
+  <si>
+    <t>LEG</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>AIN</t>
   </si>
 </sst>
 </file>
@@ -538,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,6 +791,46 @@
       </c>
       <c r="AF5" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -780,7 +844,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +1027,9 @@
       <c r="A13" s="12">
         <v>44207</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
@@ -979,7 +1045,9 @@
       <c r="A14" s="12">
         <v>44208</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
@@ -995,7 +1063,9 @@
       <c r="A15" s="12">
         <v>44209</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
@@ -1011,7 +1081,9 @@
       <c r="A16" s="12">
         <v>44210</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
@@ -1027,7 +1099,9 @@
       <c r="A17" s="12">
         <v>44211</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
@@ -1075,7 +1149,9 @@
       <c r="A20" s="12">
         <v>44214</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="6"/>
@@ -1091,7 +1167,9 @@
       <c r="A21" s="12">
         <v>44215</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="6"/>
@@ -1102,7 +1180,9 @@
       <c r="A22" s="12">
         <v>44216</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="6"/>
@@ -1113,7 +1193,9 @@
       <c r="A23" s="12">
         <v>44217</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="6"/>
@@ -1124,7 +1206,9 @@
       <c r="A24" s="12">
         <v>44218</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="6"/>
@@ -1157,7 +1241,9 @@
       <c r="A27" s="12">
         <v>44221</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="6"/>
@@ -1168,7 +1254,9 @@
       <c r="A28" s="12">
         <v>44222</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="6"/>
@@ -1179,7 +1267,9 @@
       <c r="A29" s="12">
         <v>44223</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="6"/>
@@ -1190,7 +1280,9 @@
       <c r="A30" s="12">
         <v>44224</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="6"/>
@@ -1201,7 +1293,9 @@
       <c r="A31" s="12">
         <v>44225</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="6"/>

</xml_diff>

<commit_message>
cambiata formula calcolo punteggio
</commit_message>
<xml_diff>
--- a/turniMaker/src/main/resources/dati.xlsx
+++ b/turniMaker/src/main/resources/dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cross_os\sviluppo\java_projects\SuiteTurni\turniMaker\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F95661-B861-4B73-90DB-14CC3F5AD3F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B652948-F0BC-4191-A41B-23C74A2E75DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="4425" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4425" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Persone-Indisp" sheetId="2" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
-  <si>
-    <t>BAI</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>CAR</t>
   </si>
@@ -50,15 +47,6 @@
     <t>EMA</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>GN</t>
-  </si>
-  <si>
     <t>MAR</t>
   </si>
   <si>
@@ -80,7 +68,10 @@
     <t>BOM</t>
   </si>
   <si>
-    <t>AIN</t>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>ZZZ</t>
   </si>
 </sst>
 </file>
@@ -91,8 +82,16 @@
     <numFmt numFmtId="164" formatCode="d/m;@"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -208,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,7 +244,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -564,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,167 +675,63 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -843,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,45 +755,43 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>44197</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="B3" s="16"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="6"/>
@@ -903,7 +802,7 @@
       <c r="A4" s="12">
         <v>44198</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="6"/>
@@ -914,7 +813,7 @@
       <c r="A5" s="12">
         <v>44199</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="6"/>
@@ -925,9 +824,7 @@
       <c r="A6" s="12">
         <v>44200</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B6" s="16"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="6"/>
@@ -938,9 +835,7 @@
       <c r="A7" s="12">
         <v>44201</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B7" s="16"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
@@ -951,9 +846,7 @@
       <c r="A8" s="12">
         <v>44202</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B8" s="16"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
@@ -964,9 +857,7 @@
       <c r="A9" s="12">
         <v>44203</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B9" s="16"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
@@ -977,9 +868,7 @@
       <c r="A10" s="12">
         <v>44204</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B10" s="16"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
@@ -995,7 +884,7 @@
       <c r="A11" s="12">
         <v>44205</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
@@ -1011,7 +900,7 @@
       <c r="A12" s="12">
         <v>44206</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
@@ -1027,9 +916,7 @@
       <c r="A13" s="12">
         <v>44207</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B13" s="16"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
@@ -1045,9 +932,7 @@
       <c r="A14" s="12">
         <v>44208</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B14" s="16"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
@@ -1063,9 +948,7 @@
       <c r="A15" s="12">
         <v>44209</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B15" s="16"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
@@ -1081,9 +964,7 @@
       <c r="A16" s="12">
         <v>44210</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B16" s="16"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
@@ -1099,9 +980,7 @@
       <c r="A17" s="12">
         <v>44211</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B17" s="16"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
@@ -1117,7 +996,7 @@
       <c r="A18" s="12">
         <v>44212</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="6"/>
@@ -1133,7 +1012,7 @@
       <c r="A19" s="12">
         <v>44213</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="6"/>
@@ -1149,9 +1028,7 @@
       <c r="A20" s="12">
         <v>44214</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B20" s="16"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="6"/>
@@ -1167,9 +1044,7 @@
       <c r="A21" s="12">
         <v>44215</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B21" s="16"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="6"/>
@@ -1180,9 +1055,7 @@
       <c r="A22" s="12">
         <v>44216</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B22" s="16"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="6"/>
@@ -1193,9 +1066,7 @@
       <c r="A23" s="12">
         <v>44217</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B23" s="16"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="6"/>
@@ -1206,9 +1077,7 @@
       <c r="A24" s="12">
         <v>44218</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B24" s="16"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="6"/>
@@ -1219,7 +1088,7 @@
       <c r="A25" s="12">
         <v>44219</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="6"/>
@@ -1230,7 +1099,7 @@
       <c r="A26" s="12">
         <v>44220</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="6"/>
@@ -1241,9 +1110,7 @@
       <c r="A27" s="12">
         <v>44221</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B27" s="16"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="6"/>
@@ -1254,9 +1121,7 @@
       <c r="A28" s="12">
         <v>44222</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B28" s="16"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="6"/>
@@ -1267,9 +1132,7 @@
       <c r="A29" s="12">
         <v>44223</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B29" s="16"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="6"/>
@@ -1280,9 +1143,7 @@
       <c r="A30" s="12">
         <v>44224</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B30" s="16"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="6"/>
@@ -1293,9 +1154,7 @@
       <c r="A31" s="12">
         <v>44225</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="B31" s="16"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="6"/>
@@ -1306,7 +1165,7 @@
       <c r="A32" s="12">
         <v>44226</v>
       </c>
-      <c r="B32" s="8"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="6"/>

</xml_diff>